<commit_message>
Erster Upload: EFA CHECKS Umfrage
</commit_message>
<xml_diff>
--- a/survey_results.xlsx
+++ b/survey_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,19 +473,30 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>4</t>
         </is>
       </c>
     </row>

</xml_diff>